<commit_message>
add: se actualiza el ISA y el diagrama de microarquitectura
</commit_message>
<xml_diff>
--- a/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
+++ b/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\Proyecto2_Arqui2\vectorial_cpu\ISA AND MICROARCHITECTURE\ISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2387D2FD-FBFA-4C25-9202-300A0B74C35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9BACEE-BFAB-4AEB-8D97-676D4843D859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -38,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="176">
-  <si>
-    <t>27:26</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="175">
   <si>
     <t>Control</t>
   </si>
@@ -173,12 +170,6 @@
   </si>
   <si>
     <t>NOP</t>
-  </si>
-  <si>
-    <t>00000000000000000000000000</t>
-  </si>
-  <si>
-    <t>25:0</t>
   </si>
   <si>
     <t>System</t>
@@ -1015,6 +1006,12 @@
   </si>
   <si>
     <t>Instr number</t>
+  </si>
+  <si>
+    <t>0000000000000000000000000</t>
+  </si>
+  <si>
+    <t>24:0</t>
   </si>
 </sst>
 </file>
@@ -1488,18 +1485,49 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1515,25 +1543,16 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1587,6 +1606,30 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,52 +1650,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1985,7 +1982,7 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2006,436 +2003,436 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B3" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
+      <c r="B3" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="72"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="80"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="66"/>
+        <v>170</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="74"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
+      <c r="B11" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="46" t="s">
-        <v>28</v>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="57" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="47"/>
+      <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2450,472 +2447,480 @@
     </row>
     <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
-      <c r="B25" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
+      <c r="B25" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="82" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="87"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="89" t="s">
-        <v>28</v>
+      <c r="F26" s="84"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="86" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="83" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="90"/>
+      <c r="H27" s="87"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="G28" s="84" t="s">
-        <v>168</v>
+        <v>160</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>165</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" s="7">
         <v>11</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="7">
         <v>11</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="7">
         <v>11</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="38" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="7">
         <v>11</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G32" s="38" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="E33" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="G33" s="85" t="s">
-        <v>169</v>
-      </c>
       <c r="H33" s="40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B35" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
+      <c r="B35" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="88"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="88"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="92"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="94" t="s">
+      <c r="B36" s="89" t="s">
         <v>28</v>
+      </c>
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="47"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="62" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="D37" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>28</v>
-      </c>
       <c r="E37" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="95"/>
+      <c r="H37" s="63"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G39" s="82" t="s">
-        <v>169</v>
+        <v>41</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>166</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="82" t="s">
-        <v>169</v>
+        <v>41</v>
+      </c>
+      <c r="G40" s="42" t="s">
+        <v>166</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B42" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
+      <c r="B42" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="54" t="s">
+      <c r="B43" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="55"/>
+      <c r="C43" s="90"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="52"/>
       <c r="G43" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="96" t="s">
-        <v>28</v>
+        <v>172</v>
+      </c>
+      <c r="H43" s="64" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="D44" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="57"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
       <c r="G44" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="97"/>
+        <v>18</v>
+      </c>
+      <c r="H44" s="65"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="E45" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="45"/>
+        <v>170</v>
+      </c>
+      <c r="E45" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" s="55"/>
       <c r="G45" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F46" s="42"/>
+        <v>12</v>
+      </c>
+      <c r="E46" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="49"/>
       <c r="G46" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" s="42"/>
+        <v>12</v>
+      </c>
+      <c r="E47" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="49"/>
       <c r="G47" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="42"/>
+        <v>12</v>
+      </c>
+      <c r="E48" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="49"/>
       <c r="G48" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="E9:H9"/>
@@ -2924,24 +2929,16 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E36:G36"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="E43:F44"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B43:D43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2980,91 +2977,91 @@
   <sheetData>
     <row r="1" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G2" s="25">
         <v>0</v>
       </c>
-      <c r="H2" s="77" t="s">
-        <v>61</v>
+      <c r="H2" s="93" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G3" s="25">
         <v>1</v>
       </c>
-      <c r="H3" s="77"/>
+      <c r="H3" s="93"/>
     </row>
     <row r="4" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G4" s="25">
         <v>2</v>
       </c>
-      <c r="H4" s="77"/>
+      <c r="H4" s="93"/>
     </row>
     <row r="5" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
@@ -3077,205 +3074,205 @@
     </row>
     <row r="6" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="75">
+        <v>90</v>
+      </c>
+      <c r="G6" s="91">
         <v>0</v>
       </c>
-      <c r="H6" s="75" t="s">
-        <v>60</v>
+      <c r="H6" s="91" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="78"/>
+        <v>119</v>
+      </c>
+      <c r="G7" s="92"/>
+      <c r="H7" s="94"/>
     </row>
     <row r="8" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" s="75">
+        <v>93</v>
+      </c>
+      <c r="G8" s="91">
         <v>1</v>
       </c>
-      <c r="H8" s="78"/>
+      <c r="H8" s="94"/>
     </row>
     <row r="9" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" s="76"/>
-      <c r="H9" s="78"/>
+        <v>117</v>
+      </c>
+      <c r="G9" s="92"/>
+      <c r="H9" s="94"/>
     </row>
     <row r="10" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="75">
+        <v>91</v>
+      </c>
+      <c r="G10" s="91">
         <v>2</v>
       </c>
-      <c r="H10" s="78"/>
+      <c r="H10" s="94"/>
     </row>
     <row r="11" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="78"/>
+        <v>106</v>
+      </c>
+      <c r="G11" s="92"/>
+      <c r="H11" s="94"/>
     </row>
     <row r="12" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="75">
+        <v>92</v>
+      </c>
+      <c r="G12" s="91">
         <v>3</v>
       </c>
-      <c r="H12" s="78"/>
+      <c r="H12" s="94"/>
     </row>
     <row r="13" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="76"/>
-      <c r="H13" s="78"/>
+        <v>115</v>
+      </c>
+      <c r="G13" s="92"/>
+      <c r="H13" s="94"/>
     </row>
     <row r="14" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="75">
+        <v>97</v>
+      </c>
+      <c r="G14" s="91">
         <v>4</v>
       </c>
-      <c r="H14" s="78"/>
+      <c r="H14" s="94"/>
     </row>
     <row r="15" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
+        <v>96</v>
+      </c>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
     </row>
     <row r="16" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
@@ -3288,85 +3285,85 @@
     </row>
     <row r="17" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="75">
+        <v>100</v>
+      </c>
+      <c r="G17" s="91">
         <v>0</v>
       </c>
-      <c r="H17" s="75" t="s">
-        <v>58</v>
+      <c r="H17" s="91" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="76"/>
-      <c r="H18" s="78"/>
+        <v>99</v>
+      </c>
+      <c r="G18" s="92"/>
+      <c r="H18" s="94"/>
     </row>
     <row r="19" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="75">
+        <v>101</v>
+      </c>
+      <c r="G19" s="91">
         <v>1</v>
       </c>
-      <c r="H19" s="78"/>
+      <c r="H19" s="94"/>
     </row>
     <row r="20" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
+        <v>102</v>
+      </c>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
     </row>
     <row r="21" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
@@ -3379,68 +3376,68 @@
     </row>
     <row r="22" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G22" s="25">
         <v>0</v>
       </c>
-      <c r="H22" s="77" t="s">
-        <v>57</v>
+      <c r="H22" s="93" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D23" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="34" t="s">
         <v>113</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>116</v>
       </c>
       <c r="G23" s="25">
         <v>1</v>
       </c>
-      <c r="H23" s="77"/>
+      <c r="H23" s="93"/>
     </row>
     <row r="24" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D24" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="34" t="s">
         <v>114</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="34" t="s">
-        <v>117</v>
       </c>
       <c r="G24" s="25">
         <v>2</v>
       </c>
-      <c r="H24" s="77"/>
+      <c r="H24" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3478,46 +3475,46 @@
   <sheetData>
     <row r="2" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>63</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="34" t="s">
         <v>64</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.3">
@@ -3527,57 +3524,57 @@
     </row>
     <row r="7" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.3">
@@ -3587,24 +3584,24 @@
     </row>
     <row r="13" spans="2:4" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="96.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.3">
@@ -3614,54 +3611,54 @@
     </row>
     <row r="16" spans="2:4" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="84.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20" s="79" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="79"/>
+        <v>148</v>
+      </c>
+      <c r="C20" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="95"/>
     </row>
     <row r="21" spans="2:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="81"/>
+        <v>147</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add: se agregan los algoritmos y se actualiza el isa
</commit_message>
<xml_diff>
--- a/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
+++ b/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\Proyecto2_Arqui2\vectorial_cpu\ISA AND MICROARCHITECTURE\ISA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Arqui 2\2023_ARQUI2_PROYECTO2\vectorial_cpu\ISA AND MICROARCHITECTURE\ISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9BACEE-BFAB-4AEB-8D97-676D4843D859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212F174B-590C-4BA3-B354-AD2EE9820ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -1485,7 +1485,6 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1493,6 +1492,96 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1525,24 +1614,6 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1555,78 +1626,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1650,6 +1649,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1981,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2003,41 +2005,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="75" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="77"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
@@ -2049,10 +2051,10 @@
       <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="80"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
@@ -2064,12 +2066,12 @@
       <c r="D6" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="67"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
@@ -2084,12 +2086,12 @@
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
@@ -2104,12 +2106,12 @@
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="69" t="s">
+      <c r="E8" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -2124,36 +2126,36 @@
       <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="64"/>
     </row>
     <row r="11" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="57" t="s">
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="54" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2176,7 +2178,7 @@
       <c r="G13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="58"/>
+      <c r="H13" s="55"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
@@ -2447,29 +2449,29 @@
     </row>
     <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="83" t="s">
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="84"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="86" t="s">
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2490,10 +2492,10 @@
       <c r="F27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="43" t="s">
+      <c r="G27" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="87"/>
+      <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
@@ -2512,7 +2514,7 @@
       <c r="F28" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G28" s="43" t="s">
         <v>165</v>
       </c>
       <c r="H28" s="13" t="s">
@@ -2642,7 +2644,7 @@
       <c r="F33" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="44" t="s">
         <v>166</v>
       </c>
       <c r="H33" s="40" t="s">
@@ -2650,28 +2652,28 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="88"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="89" t="s">
+      <c r="B36" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="46" t="s">
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="62" t="s">
+      <c r="F36" s="76"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="85" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2694,7 +2696,7 @@
       <c r="G37" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="63"/>
+      <c r="H37" s="86"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="16" t="s">
@@ -2738,7 +2740,7 @@
       <c r="F39" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G39" s="42" t="s">
+      <c r="G39" s="97" t="s">
         <v>166</v>
       </c>
       <c r="H39" s="6" t="s">
@@ -2764,7 +2766,7 @@
       <c r="F40" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G40" s="42" t="s">
+      <c r="G40" s="97" t="s">
         <v>166</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -2772,30 +2774,30 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="79"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="90" t="s">
+      <c r="B43" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="90"/>
-      <c r="D43" s="90"/>
-      <c r="E43" s="51" t="s">
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="52"/>
+      <c r="F43" s="81"/>
       <c r="G43" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="H43" s="64" t="s">
+      <c r="H43" s="87" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2809,12 +2811,12 @@
       <c r="D44" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="53"/>
-      <c r="F44" s="54"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="83"/>
       <c r="G44" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="65"/>
+      <c r="H44" s="88"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="19" t="s">
@@ -2826,10 +2828,10 @@
       <c r="D45" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="84" t="s">
         <v>171</v>
       </c>
-      <c r="F45" s="55"/>
+      <c r="F45" s="84"/>
       <c r="G45" s="19" t="s">
         <v>165</v>
       </c>
@@ -2850,10 +2852,10 @@
       <c r="D46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F46" s="49"/>
+      <c r="F46" s="78"/>
       <c r="G46" s="7" t="s">
         <v>166</v>
       </c>
@@ -2874,10 +2876,10 @@
       <c r="D47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="49"/>
+      <c r="F47" s="78"/>
       <c r="G47" s="7" t="s">
         <v>166</v>
       </c>
@@ -2898,10 +2900,10 @@
       <c r="D48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="49" t="s">
+      <c r="E48" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="49"/>
+      <c r="F48" s="78"/>
       <c r="G48" s="7" t="s">
         <v>166</v>
       </c>
@@ -2911,11 +2913,14 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B43:D43"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="B12:D12"/>
@@ -2929,16 +2934,13 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E45:F45"/>
     <mergeCell ref="H36:H37"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="B43:D43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3017,7 +3019,7 @@
       <c r="G2" s="25">
         <v>0</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="92" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3040,7 +3042,7 @@
       <c r="G3" s="25">
         <v>1</v>
       </c>
-      <c r="H3" s="93"/>
+      <c r="H3" s="92"/>
     </row>
     <row r="4" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
@@ -3061,7 +3063,7 @@
       <c r="G4" s="25">
         <v>2</v>
       </c>
-      <c r="H4" s="93"/>
+      <c r="H4" s="92"/>
     </row>
     <row r="5" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
@@ -3088,10 +3090,10 @@
       <c r="F6" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="91">
+      <c r="G6" s="90">
         <v>0</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="90" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3111,8 +3113,8 @@
       <c r="F7" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="92"/>
-      <c r="H7" s="94"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="93"/>
     </row>
     <row r="8" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
@@ -3130,10 +3132,10 @@
       <c r="F8" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="91">
+      <c r="G8" s="90">
         <v>1</v>
       </c>
-      <c r="H8" s="94"/>
+      <c r="H8" s="93"/>
     </row>
     <row r="9" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
@@ -3151,8 +3153,8 @@
       <c r="F9" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="92"/>
-      <c r="H9" s="94"/>
+      <c r="G9" s="91"/>
+      <c r="H9" s="93"/>
     </row>
     <row r="10" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
@@ -3170,10 +3172,10 @@
       <c r="F10" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="91">
+      <c r="G10" s="90">
         <v>2</v>
       </c>
-      <c r="H10" s="94"/>
+      <c r="H10" s="93"/>
     </row>
     <row r="11" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
@@ -3191,8 +3193,8 @@
       <c r="F11" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="94"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="93"/>
     </row>
     <row r="12" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
@@ -3210,10 +3212,10 @@
       <c r="F12" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="91">
+      <c r="G12" s="90">
         <v>3</v>
       </c>
-      <c r="H12" s="94"/>
+      <c r="H12" s="93"/>
     </row>
     <row r="13" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
@@ -3231,8 +3233,8 @@
       <c r="F13" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="92"/>
-      <c r="H13" s="94"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="93"/>
     </row>
     <row r="14" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
@@ -3250,10 +3252,10 @@
       <c r="F14" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="90">
         <v>4</v>
       </c>
-      <c r="H14" s="94"/>
+      <c r="H14" s="93"/>
     </row>
     <row r="15" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
@@ -3271,8 +3273,8 @@
       <c r="F15" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
     </row>
     <row r="16" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
@@ -3299,10 +3301,10 @@
       <c r="F17" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="91">
+      <c r="G17" s="90">
         <v>0</v>
       </c>
-      <c r="H17" s="91" t="s">
+      <c r="H17" s="90" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3322,8 +3324,8 @@
       <c r="F18" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="94"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="93"/>
     </row>
     <row r="19" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
@@ -3341,10 +3343,10 @@
       <c r="F19" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="91">
+      <c r="G19" s="90">
         <v>1</v>
       </c>
-      <c r="H19" s="94"/>
+      <c r="H19" s="93"/>
     </row>
     <row r="20" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
@@ -3362,8 +3364,8 @@
       <c r="F20" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
     </row>
     <row r="21" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
@@ -3393,7 +3395,7 @@
       <c r="G22" s="25">
         <v>0</v>
       </c>
-      <c r="H22" s="93" t="s">
+      <c r="H22" s="92" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3416,7 +3418,7 @@
       <c r="G23" s="25">
         <v>1</v>
       </c>
-      <c r="H23" s="93"/>
+      <c r="H23" s="92"/>
     </row>
     <row r="24" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
@@ -3437,7 +3439,7 @@
       <c r="G24" s="25">
         <v>2</v>
       </c>
-      <c r="H24" s="93"/>
+      <c r="H24" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3646,19 +3648,19 @@
       <c r="B20" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="95"/>
+      <c r="D20" s="94"/>
     </row>
     <row r="21" spans="2:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="97"/>
+      <c r="D21" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add: integracion completa en el proyecto vectorial aislado
</commit_message>
<xml_diff>
--- a/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
+++ b/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Arqui 2\2023_ARQUI2_PROYECTO2\vectorial_cpu\ISA AND MICROARCHITECTURE\ISA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/jeykimers_johnson_estudiantec_cr/Documents/semesters/2023 - Sem I/Arquitectura 2/project2/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212F174B-590C-4BA3-B354-AD2EE9820ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{212F174B-590C-4BA3-B354-AD2EE9820ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C0FDFF5-2555-418B-898E-34261C342B50}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="BINARY" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="184">
   <si>
     <t>Control</t>
   </si>
@@ -1012,6 +1012,33 @@
   </si>
   <si>
     <t>24:0</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>00001000</t>
+  </si>
+  <si>
+    <t>0000000000000</t>
+  </si>
+  <si>
+    <t>430C2000</t>
+  </si>
+  <si>
+    <t>R8 = R6 + R0[3]</t>
+  </si>
+  <si>
+    <t>R8 = R6 + R3</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1362,11 +1389,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1494,6 +1530,102 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1518,72 +1650,6 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1591,27 +1657,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1620,15 +1665,6 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1650,7 +1686,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1981,67 +2027,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.85" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" style="1" customWidth="1"/>
-    <col min="9" max="15" width="8.88671875" style="1"/>
-    <col min="16" max="16" width="15.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.88671875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="6.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.09765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" style="1" customWidth="1"/>
+    <col min="9" max="14" width="8.8984375" style="1"/>
+    <col min="15" max="15" width="14.3984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.09765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.8984375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+    <row r="1" spans="1:14" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B3" s="58" t="s">
+    <row r="2" spans="1:14" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:14" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B3" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="59" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+    </row>
+    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="68" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="70"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="72"/>
+    </row>
+    <row r="5" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
@@ -2051,12 +2098,12 @@
       <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="71"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="73"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
+    </row>
+    <row r="6" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="22" t="s">
         <v>2</v>
       </c>
@@ -2066,14 +2113,14 @@
       <c r="D6" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="67" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="67"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="69"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>43</v>
       </c>
@@ -2086,14 +2133,23 @@
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="64"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="99" t="str">
+        <f>_xlfn.CONCAT(B7:H7)</f>
+        <v>00000000000000000000000000000000</v>
+      </c>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+    </row>
+    <row r="8" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>45</v>
       </c>
@@ -2106,14 +2162,23 @@
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="64"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="98" t="str">
+        <f>_xlfn.CONCAT(B8:H8)</f>
+        <v>00010000000000000000000000000000</v>
+      </c>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>42</v>
       </c>
@@ -2126,40 +2191,49 @@
       <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="64"/>
-    </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="74" t="s">
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="98" t="str">
+        <f t="shared" ref="I8:I9" si="0">_xlfn.CONCAT(B9:H9)</f>
+        <v>00100000000000000000000000000000</v>
+      </c>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+    </row>
+    <row r="11" spans="1:14" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B11" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="56" t="s">
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B12" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56" t="s">
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="54" t="s">
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="56" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
@@ -2178,9 +2252,9 @@
       <c r="G13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="55"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="57"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
@@ -2203,7 +2277,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>150</v>
       </c>
@@ -2214,22 +2288,26 @@
         <v>12</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f>_xlfn.CONCAT(B15:H15)</f>
+        <v>01000010010011001100000000000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>154</v>
       </c>
@@ -2255,7 +2333,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>151</v>
       </c>
@@ -2280,8 +2358,11 @@
       <c r="H17" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>155</v>
       </c>
@@ -2306,8 +2387,11 @@
       <c r="H18" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>152</v>
       </c>
@@ -2333,7 +2417,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>156</v>
       </c>
@@ -2359,7 +2443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>153</v>
       </c>
@@ -2385,7 +2469,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>157</v>
       </c>
@@ -2411,7 +2495,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>10</v>
       </c>
@@ -2436,8 +2520,11 @@
       <c r="H23" s="40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
@@ -2447,35 +2534,35 @@
       <c r="G24" s="8"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="17.75" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+    </row>
+    <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46" t="s">
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49" t="s">
+      <c r="F26" s="79"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="81" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="12" t="s">
         <v>1</v>
@@ -2495,9 +2582,9 @@
       <c r="G27" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="50"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="82"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="13" t="s">
         <v>2</v>
@@ -2521,7 +2608,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>150</v>
       </c>
@@ -2534,20 +2621,20 @@
       <c r="D29" s="7">
         <v>11</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G29" s="38" t="s">
-        <v>166</v>
+      <c r="E29" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="103" t="s">
+        <v>179</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>151</v>
       </c>
@@ -2573,7 +2660,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>152</v>
       </c>
@@ -2599,7 +2686,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>153</v>
       </c>
@@ -2625,7 +2712,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="39" t="s">
         <v>10</v>
       </c>
@@ -2651,33 +2738,33 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B35" s="51" t="s">
+    <row r="35" spans="1:12" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B35" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="52" t="s">
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+    </row>
+    <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B36" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="75" t="s">
+      <c r="C36" s="84"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="76"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="85" t="s">
+      <c r="F36" s="86"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="88" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
         <v>25</v>
       </c>
@@ -2696,9 +2783,9 @@
       <c r="G37" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="86"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="89"/>
+    </row>
+    <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B38" s="16" t="s">
         <v>2</v>
       </c>
@@ -2721,7 +2808,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>20</v>
       </c>
@@ -2734,20 +2821,27 @@
       <c r="D39" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G39" s="97" t="s">
-        <v>166</v>
+      <c r="E39" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="103" t="s">
+        <v>179</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="101" t="str">
+        <f>_xlfn.CONCAT(B39:H39)</f>
+        <v>10000000101100000001000000000000</v>
+      </c>
+      <c r="J39" s="102"/>
+      <c r="K39" s="102"/>
+      <c r="L39" s="102"/>
+    </row>
+    <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>21</v>
       </c>
@@ -2760,48 +2854,55 @@
       <c r="D40" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G40" s="97" t="s">
-        <v>166</v>
+      <c r="E40" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="103" t="s">
+        <v>179</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B42" s="79" t="s">
+      <c r="I40" s="101" t="str">
+        <f>_xlfn.CONCAT(B40:H40)</f>
+        <v>10100000110100000001000000000000</v>
+      </c>
+      <c r="J40" s="102"/>
+      <c r="K40" s="102"/>
+      <c r="L40" s="102"/>
+    </row>
+    <row r="42" spans="1:12" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B42" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="79"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="79"/>
-      <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="89" t="s">
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+    </row>
+    <row r="43" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B43" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="89"/>
-      <c r="D43" s="89"/>
-      <c r="E43" s="80" t="s">
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="81"/>
+      <c r="F43" s="48"/>
       <c r="G43" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="H43" s="87" t="s">
+      <c r="H43" s="52" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="18" t="s">
         <v>25</v>
       </c>
@@ -2811,14 +2912,14 @@
       <c r="D44" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="82"/>
-      <c r="F44" s="83"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="88"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="53"/>
+    </row>
+    <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B45" s="19" t="s">
         <v>2</v>
       </c>
@@ -2828,10 +2929,10 @@
       <c r="D45" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="E45" s="84" t="s">
+      <c r="E45" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="F45" s="84"/>
+      <c r="F45" s="51"/>
       <c r="G45" s="19" t="s">
         <v>165</v>
       </c>
@@ -2839,7 +2940,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
         <v>3</v>
       </c>
@@ -2852,10 +2953,10 @@
       <c r="D46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="78" t="s">
+      <c r="E46" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F46" s="78"/>
+      <c r="F46" s="45"/>
       <c r="G46" s="7" t="s">
         <v>166</v>
       </c>
@@ -2863,7 +2964,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>4</v>
       </c>
@@ -2876,10 +2977,10 @@
       <c r="D47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="78" t="s">
+      <c r="E47" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="78"/>
+      <c r="F47" s="45"/>
       <c r="G47" s="7" t="s">
         <v>166</v>
       </c>
@@ -2887,7 +2988,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
         <v>48</v>
       </c>
@@ -2900,10 +3001,10 @@
       <c r="D48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="78" t="s">
+      <c r="E48" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="78"/>
+      <c r="F48" s="45"/>
       <c r="G48" s="7" t="s">
         <v>166</v>
       </c>
@@ -2912,15 +3013,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="B43:D43"/>
+  <mergeCells count="33">
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:H37"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="B12:D12"/>
@@ -2934,13 +3039,14 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B43:D43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2958,23 +3064,23 @@
   </sheetPr>
   <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="40" zoomScaleNormal="55" zoomScalePageLayoutView="40" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A12" zoomScale="114" zoomScaleNormal="55" zoomScalePageLayoutView="114" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="24"/>
-    <col min="8" max="8" width="10.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="24" customWidth="1"/>
-    <col min="10" max="10" width="67.44140625" style="24" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="24"/>
+    <col min="1" max="1" width="14.3984375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="15.296875" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3984375" style="24" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.09765625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.59765625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="14.3984375" style="24"/>
+    <col min="8" max="8" width="10.69921875" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" style="24" customWidth="1"/>
+    <col min="10" max="10" width="67.3984375" style="24" customWidth="1"/>
+    <col min="11" max="16384" width="14.3984375" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3065,7 +3171,7 @@
       </c>
       <c r="H4" s="92"/>
     </row>
-    <row r="5" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -3276,7 +3382,7 @@
       <c r="G15" s="91"/>
       <c r="H15" s="91"/>
     </row>
-    <row r="16" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -3367,7 +3473,7 @@
       <c r="G20" s="91"/>
       <c r="H20" s="91"/>
     </row>
-    <row r="21" spans="2:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
@@ -3399,7 +3505,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
         <v>4</v>
       </c>
@@ -3470,12 +3576,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="80.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" customWidth="1"/>
+    <col min="4" max="4" width="80.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="27.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="33" t="s">
         <v>52</v>
       </c>
@@ -3486,7 +3592,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
         <v>43</v>
       </c>
@@ -3519,12 +3625,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="14.95" x14ac:dyDescent="0.3">
       <c r="B6" s="27"/>
       <c r="C6" s="36"/>
       <c r="D6" s="28"/>
     </row>
-    <row r="7" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
         <v>8</v>
       </c>
@@ -3535,7 +3641,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="25" t="s">
         <v>9</v>
       </c>
@@ -3546,7 +3652,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="25" t="s">
         <v>40</v>
       </c>
@@ -3557,7 +3663,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="25" t="s">
         <v>47</v>
       </c>
@@ -3568,7 +3674,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25" t="s">
         <v>10</v>
       </c>
@@ -3579,12 +3685,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="14.95" x14ac:dyDescent="0.3">
       <c r="B12" s="27"/>
       <c r="C12" s="36"/>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="2:4" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" ht="101.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
         <v>20</v>
       </c>
@@ -3595,7 +3701,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="96.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="96.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="25" t="s">
         <v>21</v>
       </c>
@@ -3606,7 +3712,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="14.95" x14ac:dyDescent="0.3">
       <c r="B15" s="27"/>
       <c r="C15" s="36"/>
       <c r="D15" s="28"/>
@@ -3622,7 +3728,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="84.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="84.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="25" t="s">
         <v>4</v>
       </c>
@@ -3633,7 +3739,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="85.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="25" t="s">
         <v>48</v>
       </c>
@@ -3644,7 +3750,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" ht="27.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="37" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
add: load escalar con bandera VSIFlag
</commit_message>
<xml_diff>
--- a/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
+++ b/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/jeykimers_johnson_estudiantec_cr/Documents/semesters/2023 - Sem I/Arquitectura 2/project2/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{212F174B-590C-4BA3-B354-AD2EE9820ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C0FDFF5-2555-418B-898E-34261C342B50}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{212F174B-590C-4BA3-B354-AD2EE9820ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A685489-C186-4901-9EB3-70C25529EE38}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
+    <workbookView xWindow="2238" yWindow="565" windowWidth="15950" windowHeight="8673" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="BINARY" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="185">
   <si>
     <t>Control</t>
   </si>
@@ -1023,9 +1023,6 @@
     <t>0110</t>
   </si>
   <si>
-    <t>0101</t>
-  </si>
-  <si>
     <t>00001000</t>
   </si>
   <si>
@@ -1039,6 +1036,12 @@
   </si>
   <si>
     <t>R8 = R6 + R3</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>00000100</t>
   </si>
 </sst>
 </file>
@@ -1531,6 +1534,124 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1560,111 +1681,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1685,19 +1701,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1728,6 +1731,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2029,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.85" x14ac:dyDescent="0.25"/>
@@ -2052,41 +2059,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:14" ht="17.75" x14ac:dyDescent="0.35">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
     </row>
     <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="70" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
@@ -2098,10 +2105,10 @@
       <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="75"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="85"/>
     </row>
     <row r="6" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="22" t="s">
@@ -2113,12 +2120,12 @@
       <c r="D6" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="69"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="79"/>
     </row>
     <row r="7" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
@@ -2133,21 +2140,21 @@
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="99" t="str">
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="46" t="str">
         <f>_xlfn.CONCAT(B7:H7)</f>
         <v>00000000000000000000000000000000</v>
       </c>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
@@ -2162,21 +2169,21 @@
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="64" t="s">
+      <c r="E8" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="98" t="str">
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="48" t="str">
         <f>_xlfn.CONCAT(B8:H8)</f>
         <v>00010000000000000000000000000000</v>
       </c>
-      <c r="J8" s="97"/>
-      <c r="K8" s="97"/>
-      <c r="L8" s="97"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="97"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
     </row>
     <row r="9" spans="1:14" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -2191,45 +2198,45 @@
       <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="98" t="str">
-        <f t="shared" ref="I8:I9" si="0">_xlfn.CONCAT(B9:H9)</f>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="48" t="str">
+        <f t="shared" ref="I9" si="0">_xlfn.CONCAT(B9:H9)</f>
         <v>00100000000000000000000000000000</v>
       </c>
-      <c r="J9" s="97"/>
-      <c r="K9" s="97"/>
-      <c r="L9" s="97"/>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
     </row>
     <row r="11" spans="1:14" ht="17.75" x14ac:dyDescent="0.35">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
     </row>
     <row r="12" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58" t="s">
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="56" t="s">
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="66" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2252,7 +2259,7 @@
       <c r="G13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="57"/>
+      <c r="H13" s="67"/>
     </row>
     <row r="14" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
@@ -2300,7 +2307,7 @@
         <v>177</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J15" s="1" t="str">
         <f>_xlfn.CONCAT(B15:H15)</f>
@@ -2359,7 +2366,7 @@
         <v>38</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -2388,7 +2395,7 @@
         <v>38</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -2521,7 +2528,7 @@
         <v>38</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -2536,29 +2543,29 @@
     </row>
     <row r="25" spans="1:11" ht="17.75" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
     </row>
     <row r="26" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="78" t="s">
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="79"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="81" t="s">
+      <c r="F26" s="54"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2582,7 +2589,7 @@
       <c r="G27" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="82"/>
+      <c r="H27" s="57"/>
     </row>
     <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
@@ -2627,8 +2634,8 @@
       <c r="F29" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G29" s="103" t="s">
-        <v>179</v>
+      <c r="G29" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>168</v>
@@ -2739,28 +2746,28 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="17.75" x14ac:dyDescent="0.35">
-      <c r="B35" s="83" t="s">
+      <c r="B35" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
     </row>
     <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="84"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="85" t="s">
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="86"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="88" t="s">
+      <c r="F36" s="61"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="63" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2783,7 +2790,7 @@
       <c r="G37" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H37" s="89"/>
+      <c r="H37" s="64"/>
     </row>
     <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B38" s="16" t="s">
@@ -2822,24 +2829,24 @@
         <v>36</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="103" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="G39" s="45" t="s">
+        <v>184</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="I39" s="101" t="str">
+      <c r="I39" s="50" t="str">
         <f>_xlfn.CONCAT(B39:H39)</f>
-        <v>10000000101100000001000000000000</v>
-      </c>
-      <c r="J39" s="102"/>
-      <c r="K39" s="102"/>
-      <c r="L39" s="102"/>
+        <v>10000000110011100000100000000000</v>
+      </c>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
     </row>
     <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
@@ -2860,45 +2867,45 @@
       <c r="F40" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G40" s="103" t="s">
-        <v>179</v>
+      <c r="G40" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="I40" s="101" t="str">
+      <c r="I40" s="50" t="str">
         <f>_xlfn.CONCAT(B40:H40)</f>
         <v>10100000110100000001000000000000</v>
       </c>
-      <c r="J40" s="102"/>
-      <c r="K40" s="102"/>
-      <c r="L40" s="102"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
     </row>
     <row r="42" spans="1:12" ht="17.75" x14ac:dyDescent="0.35">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="88"/>
+      <c r="H42" s="88"/>
     </row>
     <row r="43" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="47" t="s">
+      <c r="C43" s="96"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="48"/>
+      <c r="F43" s="90"/>
       <c r="G43" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="H43" s="52" t="s">
+      <c r="H43" s="94" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2912,12 +2919,12 @@
       <c r="D44" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="49"/>
-      <c r="F44" s="50"/>
+      <c r="E44" s="91"/>
+      <c r="F44" s="92"/>
       <c r="G44" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H44" s="53"/>
+      <c r="H44" s="95"/>
     </row>
     <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B45" s="19" t="s">
@@ -2929,10 +2936,10 @@
       <c r="D45" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="F45" s="51"/>
+      <c r="F45" s="93"/>
       <c r="G45" s="19" t="s">
         <v>165</v>
       </c>
@@ -2953,10 +2960,10 @@
       <c r="D46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="45" t="s">
+      <c r="E46" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="F46" s="45"/>
+      <c r="F46" s="87"/>
       <c r="G46" s="7" t="s">
         <v>166</v>
       </c>
@@ -2977,10 +2984,10 @@
       <c r="D47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="45" t="s">
+      <c r="E47" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="45"/>
+      <c r="F47" s="87"/>
       <c r="G47" s="7" t="s">
         <v>166</v>
       </c>
@@ -3001,10 +3008,10 @@
       <c r="D48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="45" t="s">
+      <c r="E48" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="45"/>
+      <c r="F48" s="87"/>
       <c r="G48" s="7" t="s">
         <v>166</v>
       </c>
@@ -3014,18 +3021,14 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="I39:L39"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B43:D43"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="B12:D12"/>
@@ -3039,14 +3042,18 @@
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="I40:L40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3125,7 +3132,7 @@
       <c r="G2" s="25">
         <v>0</v>
       </c>
-      <c r="H2" s="92" t="s">
+      <c r="H2" s="99" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3148,7 +3155,7 @@
       <c r="G3" s="25">
         <v>1</v>
       </c>
-      <c r="H3" s="92"/>
+      <c r="H3" s="99"/>
     </row>
     <row r="4" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
@@ -3169,7 +3176,7 @@
       <c r="G4" s="25">
         <v>2</v>
       </c>
-      <c r="H4" s="92"/>
+      <c r="H4" s="99"/>
     </row>
     <row r="5" spans="2:8" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
@@ -3196,10 +3203,10 @@
       <c r="F6" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="90">
+      <c r="G6" s="97">
         <v>0</v>
       </c>
-      <c r="H6" s="90" t="s">
+      <c r="H6" s="97" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3219,8 +3226,8 @@
       <c r="F7" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="91"/>
-      <c r="H7" s="93"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="100"/>
     </row>
     <row r="8" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
@@ -3238,10 +3245,10 @@
       <c r="F8" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="90">
+      <c r="G8" s="97">
         <v>1</v>
       </c>
-      <c r="H8" s="93"/>
+      <c r="H8" s="100"/>
     </row>
     <row r="9" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
@@ -3259,8 +3266,8 @@
       <c r="F9" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="G9" s="91"/>
-      <c r="H9" s="93"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="100"/>
     </row>
     <row r="10" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
@@ -3278,10 +3285,10 @@
       <c r="F10" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="90">
+      <c r="G10" s="97">
         <v>2</v>
       </c>
-      <c r="H10" s="93"/>
+      <c r="H10" s="100"/>
     </row>
     <row r="11" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
@@ -3299,8 +3306,8 @@
       <c r="F11" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="91"/>
-      <c r="H11" s="93"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="100"/>
     </row>
     <row r="12" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
@@ -3318,10 +3325,10 @@
       <c r="F12" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="90">
+      <c r="G12" s="97">
         <v>3</v>
       </c>
-      <c r="H12" s="93"/>
+      <c r="H12" s="100"/>
     </row>
     <row r="13" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
@@ -3339,8 +3346,8 @@
       <c r="F13" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="91"/>
-      <c r="H13" s="93"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="100"/>
     </row>
     <row r="14" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
@@ -3358,10 +3365,10 @@
       <c r="F14" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="G14" s="90">
+      <c r="G14" s="97">
         <v>4</v>
       </c>
-      <c r="H14" s="93"/>
+      <c r="H14" s="100"/>
     </row>
     <row r="15" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
@@ -3379,8 +3386,8 @@
       <c r="F15" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
     </row>
     <row r="16" spans="2:8" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
@@ -3407,10 +3414,10 @@
       <c r="F17" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="90">
+      <c r="G17" s="97">
         <v>0</v>
       </c>
-      <c r="H17" s="90" t="s">
+      <c r="H17" s="97" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3430,8 +3437,8 @@
       <c r="F18" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="91"/>
-      <c r="H18" s="93"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="100"/>
     </row>
     <row r="19" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
@@ -3449,10 +3456,10 @@
       <c r="F19" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="90">
+      <c r="G19" s="97">
         <v>1</v>
       </c>
-      <c r="H19" s="93"/>
+      <c r="H19" s="100"/>
     </row>
     <row r="20" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
@@ -3470,8 +3477,8 @@
       <c r="F20" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="98"/>
     </row>
     <row r="21" spans="2:8" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
@@ -3501,7 +3508,7 @@
       <c r="G22" s="25">
         <v>0</v>
       </c>
-      <c r="H22" s="92" t="s">
+      <c r="H22" s="99" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3524,7 +3531,7 @@
       <c r="G23" s="25">
         <v>1</v>
       </c>
-      <c r="H23" s="92"/>
+      <c r="H23" s="99"/>
     </row>
     <row r="24" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
@@ -3545,7 +3552,7 @@
       <c r="G24" s="25">
         <v>2</v>
       </c>
-      <c r="H24" s="92"/>
+      <c r="H24" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3754,19 +3761,19 @@
       <c r="B20" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="94" t="s">
+      <c r="C20" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="94"/>
+      <c r="D20" s="101"/>
     </row>
     <row r="21" spans="2:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="96"/>
+      <c r="D21" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add:  ROTATE O CIRCULAR SHIFT  terminado
</commit_message>
<xml_diff>
--- a/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
+++ b/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/ISA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Arqui 2\2023_ARQUI2_PROYECTO2\vectorial_cpu\ISA AND MICROARCHITECTURE\ISA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/jeykimers_johnson_estudiantec_cr/Documents/semesters/2023 - Sem I/Arquitectura 2/project2/vectorial_cpu/ISA AND MICROARCHITECTURE/ISA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC96D53-7311-4628-BD2A-762997BC885C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:1_{AEC96D53-7311-4628-BD2A-762997BC885C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B47A1F24-7463-4DCB-B05E-BBC617E1D351}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="BINARY" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="227">
   <si>
     <t>Control</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>00000000</t>
   </si>
   <si>
     <t>00000000000000</t>
@@ -574,18 +571,6 @@
     <t>27:25</t>
   </si>
   <si>
-    <t>24:17</t>
-  </si>
-  <si>
-    <t>Instr number</t>
-  </si>
-  <si>
-    <t>0000000000000000000000000</t>
-  </si>
-  <si>
-    <t>24:0</t>
-  </si>
-  <si>
     <t>LDRV</t>
   </si>
   <si>
@@ -1224,6 +1209,45 @@
   </si>
   <si>
     <t>Esta instrucción realiza la operación de desplazamiento a la izquierda en un valor y lo almacena en un registro destino.</t>
+  </si>
+  <si>
+    <t>16:0</t>
+  </si>
+  <si>
+    <t>00000000000000000</t>
+  </si>
+  <si>
+    <t>0000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>27:0</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>SEL</t>
+  </si>
+  <si>
+    <t>00000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>25:0</t>
+  </si>
+  <si>
+    <t>27:26</t>
+  </si>
+  <si>
+    <t>Imm</t>
+  </si>
+  <si>
+    <t>Null / Addressing</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>0000</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1554,11 +1578,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1646,9 +1732,6 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1703,6 +1786,120 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1712,40 +1909,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1757,50 +1927,11 @@
     <xf numFmtId="49" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1818,12 +1949,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1861,6 +1986,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2160,72 +2289,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.85" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" style="1" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="1"/>
-    <col min="16" max="16" width="15.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.88671875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.09765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.8984375" style="1" customWidth="1"/>
+    <col min="10" max="15" width="8.8984375" style="1"/>
+    <col min="16" max="16" width="15.09765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.296875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.8984375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+    <row r="1" spans="1:10" ht="20.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="87" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="89"/>
     </row>
     <row r="2" spans="1:10" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B3" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+    <row r="3" spans="1:10" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B3" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="85"/>
+      <c r="D4" s="86" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>21</v>
       </c>
@@ -2233,35 +2362,37 @@
         <v>22</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="E5" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="84"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-    </row>
-    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+    </row>
+    <row r="7" spans="1:10" ht="13.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -2270,19 +2401,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+    </row>
+    <row r="8" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>37</v>
+        <v>218</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>5</v>
@@ -2291,19 +2422,19 @@
         <v>6</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>34</v>
+        <v>219</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>5</v>
@@ -2312,1243 +2443,1222 @@
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-    </row>
-    <row r="11" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="52"/>
+    </row>
+    <row r="12" spans="1:10" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B12" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="93"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76" t="s">
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="66" t="s">
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="66"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="I13" s="94"/>
+    </row>
+    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H15" s="95" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" s="67"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="53"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="95"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="53"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="54"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="53"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="54"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="53"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="54"/>
+    </row>
+    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="53"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H19" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="54"/>
+    </row>
+    <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I20" s="53"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H20" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="54"/>
+    </row>
+    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="38" t="s">
+      <c r="C21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="57"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="33"/>
-    </row>
-    <row r="23" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B23" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="68" t="s">
+      <c r="E21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="54"/>
+    </row>
+    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="78"/>
+    </row>
+    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="1:9" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B24" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+    </row>
+    <row r="25" spans="1:9" ht="16.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68" t="s">
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="70" t="s">
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="70"/>
-    </row>
-    <row r="25" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="I25" s="80"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C26" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="36" t="s">
+      <c r="D26" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F26" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G26" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="H26" s="80"/>
+      <c r="I26" s="80"/>
+    </row>
+    <row r="27" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C27" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D27" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="F27" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="G27" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="H27" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="H26" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="71"/>
-    </row>
-    <row r="27" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="53"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
-        <v>103</v>
+      <c r="I27" s="81"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>101</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I28" s="53"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>123</v>
+        <v>32</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="54"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="34" t="s">
+        <v>102</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="53"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
-        <v>129</v>
+        <v>32</v>
+      </c>
+      <c r="H29" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="54"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="34" t="s">
+        <v>118</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="53"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
-        <v>132</v>
+        <v>32</v>
+      </c>
+      <c r="H30" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="54"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>124</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="53"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
-        <v>133</v>
+        <v>32</v>
+      </c>
+      <c r="H31" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="54"/>
+    </row>
+    <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="53"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>136</v>
+        <v>32</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="54"/>
+    </row>
+    <row r="33" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="34" t="s">
+        <v>128</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>33</v>
+      <c r="E33" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H33" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="53"/>
-    </row>
-    <row r="34" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="33"/>
-    </row>
-    <row r="35" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="82" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="82"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-      <c r="H35" s="82"/>
-      <c r="I35" s="82"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="54"/>
+    </row>
+    <row r="34" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="54"/>
+    </row>
+    <row r="35" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="40"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="32"/>
+    </row>
+    <row r="36" spans="1:9" ht="17.75" x14ac:dyDescent="0.35">
       <c r="A36" s="7"/>
-      <c r="B36" s="80" t="s">
+      <c r="B36" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="92"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="92"/>
+      <c r="H36" s="92"/>
+      <c r="I36" s="92"/>
+    </row>
+    <row r="37" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="81" t="s">
+      <c r="C37" s="90"/>
+      <c r="D37" s="90"/>
+      <c r="E37" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="55" t="s">
+      <c r="F37" s="91"/>
+      <c r="G37" s="91"/>
+      <c r="H37" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="55"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="43" t="s">
+      <c r="I37" s="63"/>
+    </row>
+    <row r="38" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C38" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="43" t="s">
+      <c r="D38" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+    </row>
+    <row r="39" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="F38" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="G38" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="H38" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="I38" s="56"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="6">
-        <v>11</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="6" t="s">
+      <c r="H39" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="H39" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I39" s="53"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="42" t="s">
-        <v>103</v>
+      <c r="I39" s="64"/>
+    </row>
+    <row r="40" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="41" t="s">
+        <v>101</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40" s="6">
         <v>11</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H40" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I40" s="53"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="42" t="s">
-        <v>123</v>
+        <v>110</v>
+      </c>
+      <c r="H40" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" s="54"/>
+    </row>
+    <row r="41" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="41" t="s">
+        <v>102</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41" s="6">
         <v>11</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>33</v>
+        <v>226</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H41" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I41" s="53"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="s">
-        <v>129</v>
+        <v>110</v>
+      </c>
+      <c r="H41" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I41" s="54"/>
+    </row>
+    <row r="42" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="41" t="s">
+        <v>118</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D42" s="6">
         <v>11</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H42" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I42" s="53"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="42" t="s">
-        <v>132</v>
+        <v>110</v>
+      </c>
+      <c r="H42" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I42" s="54"/>
+    </row>
+    <row r="43" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="41" t="s">
+        <v>124</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="6">
         <v>11</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>33</v>
+      <c r="E43" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H43" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I43" s="53"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="42" t="s">
-        <v>133</v>
+        <v>110</v>
+      </c>
+      <c r="H43" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I43" s="54"/>
+    </row>
+    <row r="44" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="41" t="s">
+        <v>127</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="D44" s="6">
         <v>11</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H44" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I44" s="53"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="42" t="s">
-        <v>136</v>
+        <v>110</v>
+      </c>
+      <c r="H44" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I44" s="54"/>
+    </row>
+    <row r="45" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="41" t="s">
+        <v>128</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="38" t="s">
-        <v>128</v>
+      <c r="C45" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="D45" s="6">
         <v>11</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" s="54"/>
+    </row>
+    <row r="46" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" s="6">
+        <v>11</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="I46" s="54"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="32"/>
+    </row>
+    <row r="48" spans="1:9" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B48" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="61"/>
+    </row>
+    <row r="50" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B50" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H50" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="58"/>
+    </row>
+    <row r="51" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B51" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I45" s="53"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="33"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="33"/>
-    </row>
-    <row r="47" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B47" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="61"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="G48" s="59"/>
-      <c r="H48" s="60"/>
-      <c r="I48" s="78" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I49" s="79"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E50" s="9" t="s">
+      <c r="F51" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="G51" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G50" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="I50" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D51" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H51" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="I51" s="50"/>
+    </row>
+    <row r="52" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D52" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="47" t="s">
         <v>5</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H52" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H52" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="I52" s="52"/>
+    </row>
+    <row r="53" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H53" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H53" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="I53" s="52"/>
+    </row>
+    <row r="54" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H54" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="I54" s="52"/>
+    </row>
+    <row r="55" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F54" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H54" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="45"/>
-    </row>
-    <row r="56" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B56" s="54" t="s">
+      <c r="F55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="I55" s="52"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D56" s="44"/>
+    </row>
+    <row r="57" spans="1:9" ht="17.75" x14ac:dyDescent="0.35">
+      <c r="B57" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54"/>
-      <c r="E56" s="54"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="54"/>
-      <c r="H56" s="54"/>
-      <c r="I56" s="54"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="74" t="s">
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="62"/>
+      <c r="I57" s="62"/>
+    </row>
+    <row r="58" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B58" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="74"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="F57" s="72"/>
-      <c r="G57" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H57" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="I57" s="75"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="11" t="s">
+      <c r="C58" s="68"/>
+      <c r="D58" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="71"/>
+    </row>
+    <row r="59" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B59" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C59" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D58" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E58" s="72"/>
-      <c r="F58" s="72"/>
-      <c r="G58" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="75"/>
-      <c r="I58" s="75"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="12" t="s">
+      <c r="D59" s="72"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="74"/>
+    </row>
+    <row r="60" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B60" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E59" s="73" t="s">
-        <v>115</v>
-      </c>
-      <c r="F59" s="73"/>
-      <c r="G59" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="H59" s="73" t="s">
-        <v>112</v>
-      </c>
-      <c r="I59" s="73"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="C60" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="75" t="s">
+        <v>217</v>
+      </c>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="77"/>
+    </row>
+    <row r="61" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
         <v>3</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="F60" s="53"/>
-      <c r="G60" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H60" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I60" s="53"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>4</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="F61" s="53"/>
-      <c r="G61" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H61" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I61" s="53"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D61" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="E61" s="55"/>
+      <c r="F61" s="55"/>
+      <c r="G61" s="55"/>
+      <c r="H61" s="55"/>
+      <c r="I61" s="52"/>
+    </row>
+    <row r="62" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="52"/>
+    </row>
+    <row r="63" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="F62" s="53"/>
-      <c r="G62" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H62" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I62" s="53"/>
+      <c r="D63" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
+      <c r="I63" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="62">
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D63:I63"/>
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="H57:I58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B36:I36"/>
     <mergeCell ref="H28:I28"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E57:F58"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="H24:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="H13:I14"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E4:I5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="H36:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B47:I47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
     <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D61:I61"/>
+    <mergeCell ref="D60:I60"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:I59"/>
     <mergeCell ref="B3:I3"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="D62:I62"/>
+    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="H37:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H46:I46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3563,114 +3673,114 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="67.44140625" style="17" customWidth="1"/>
-    <col min="11" max="16384" width="14.44140625" style="17"/>
+    <col min="1" max="1" width="19.69921875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.3984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.59765625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.69921875" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="67.3984375" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="14.3984375" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="F1" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="46">
+      <c r="C2" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="45">
         <v>0</v>
       </c>
-      <c r="G2" s="89" t="s">
-        <v>49</v>
+      <c r="G2" s="96" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="18">
         <v>1</v>
       </c>
-      <c r="G3" s="89"/>
+      <c r="G3" s="96"/>
     </row>
     <row r="4" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="46">
+      <c r="A4" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="45">
         <v>2</v>
       </c>
-      <c r="G4" s="89"/>
-    </row>
-    <row r="5" spans="1:7" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="96"/>
+    </row>
+    <row r="5" spans="1:7" ht="13.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -3680,419 +3790,419 @@
       <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="47" t="s">
+      <c r="A6" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="97">
+        <v>0</v>
+      </c>
+      <c r="G6" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="90">
-        <v>0</v>
-      </c>
-      <c r="G6" s="83" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="7" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="90"/>
-      <c r="G7" s="84"/>
+      <c r="A7" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="97"/>
+      <c r="G7" s="99"/>
     </row>
     <row r="8" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="90"/>
-      <c r="G8" s="84"/>
+      <c r="A8" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="97"/>
+      <c r="G8" s="99"/>
     </row>
     <row r="9" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="83">
+        <v>63</v>
+      </c>
+      <c r="F9" s="98">
         <v>1</v>
       </c>
-      <c r="G9" s="84"/>
+      <c r="G9" s="99"/>
     </row>
     <row r="10" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
+        <v>63</v>
+      </c>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
     </row>
     <row r="11" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="84"/>
+        <v>136</v>
+      </c>
+      <c r="F11" s="100"/>
+      <c r="G11" s="99"/>
     </row>
     <row r="12" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="F12" s="86">
+      <c r="A12" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="101">
         <v>2</v>
       </c>
-      <c r="G12" s="84"/>
+      <c r="G12" s="99"/>
     </row>
     <row r="13" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="84"/>
+      <c r="A13" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="102"/>
+      <c r="G13" s="99"/>
     </row>
     <row r="14" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="D14" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="87"/>
-      <c r="G14" s="84"/>
+      <c r="A14" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="102"/>
+      <c r="G14" s="99"/>
     </row>
     <row r="15" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="F15" s="83">
+        <v>159</v>
+      </c>
+      <c r="F15" s="98">
         <v>3</v>
       </c>
-      <c r="G15" s="84"/>
+      <c r="G15" s="99"/>
     </row>
     <row r="16" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
+        <v>159</v>
+      </c>
+      <c r="F16" s="99"/>
+      <c r="G16" s="99"/>
     </row>
     <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F17" s="85"/>
-      <c r="G17" s="84"/>
+        <v>160</v>
+      </c>
+      <c r="F17" s="100"/>
+      <c r="G17" s="99"/>
     </row>
     <row r="18" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="101">
+        <v>4</v>
+      </c>
+      <c r="G18" s="99"/>
+    </row>
+    <row r="19" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="F18" s="86">
-        <v>4</v>
-      </c>
-      <c r="G18" s="84"/>
-    </row>
-    <row r="19" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="F19" s="87"/>
-      <c r="G19" s="84"/>
+      <c r="B19" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="102"/>
+      <c r="G19" s="99"/>
     </row>
     <row r="20" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>188</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="F20" s="88"/>
-      <c r="G20" s="84"/>
-    </row>
-    <row r="21" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="103"/>
+      <c r="G20" s="99"/>
+    </row>
+    <row r="21" spans="1:7" ht="21.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="F21" s="83">
+        <v>161</v>
+      </c>
+      <c r="F21" s="98">
         <v>5</v>
       </c>
-      <c r="G21" s="84"/>
+      <c r="G21" s="99"/>
     </row>
     <row r="22" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
+        <v>161</v>
+      </c>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
     </row>
     <row r="23" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="F23" s="85"/>
-      <c r="G23" s="84"/>
-    </row>
-    <row r="24" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="F24" s="86">
+        <v>162</v>
+      </c>
+      <c r="F23" s="100"/>
+      <c r="G23" s="99"/>
+    </row>
+    <row r="24" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="101">
         <v>6</v>
       </c>
-      <c r="G24" s="84"/>
+      <c r="G24" s="99"/>
     </row>
     <row r="25" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="47" t="s">
-        <v>204</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="F25" s="87"/>
-      <c r="G25" s="84"/>
+      <c r="A25" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="102"/>
+      <c r="G25" s="99"/>
     </row>
     <row r="26" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="47" t="s">
-        <v>192</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>171</v>
-      </c>
-      <c r="F26" s="88"/>
-      <c r="G26" s="85"/>
+      <c r="A26" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="F26" s="103"/>
+      <c r="G26" s="100"/>
     </row>
     <row r="27" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
@@ -4105,123 +4215,123 @@
     </row>
     <row r="28" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="89">
+        <v>67</v>
+      </c>
+      <c r="F28" s="96">
         <v>0</v>
       </c>
-      <c r="G28" s="83" t="s">
-        <v>46</v>
+      <c r="G28" s="98" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" s="89"/>
-      <c r="G29" s="84"/>
+        <v>170</v>
+      </c>
+      <c r="F29" s="96"/>
+      <c r="G29" s="99"/>
     </row>
     <row r="30" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="89"/>
-      <c r="G30" s="84"/>
+        <v>67</v>
+      </c>
+      <c r="F30" s="96"/>
+      <c r="G30" s="99"/>
     </row>
     <row r="31" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B31" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="96"/>
+      <c r="G31" s="99"/>
+    </row>
+    <row r="32" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="D31" s="19" t="s">
+      <c r="E32" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="101">
+        <v>1</v>
+      </c>
+      <c r="G32" s="99"/>
+    </row>
+    <row r="33" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" s="89"/>
-      <c r="G31" s="84"/>
-    </row>
-    <row r="32" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="86">
-        <v>1</v>
-      </c>
-      <c r="G32" s="84"/>
-    </row>
-    <row r="33" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="D33" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="84"/>
+      <c r="E33" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33" s="103"/>
+      <c r="G33" s="99"/>
     </row>
     <row r="34" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
@@ -4233,26 +4343,26 @@
       <c r="G34" s="25"/>
     </row>
     <row r="35" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="F35" s="46">
+      <c r="B35" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" s="45">
         <v>0</v>
       </c>
-      <c r="G35" s="89" t="s">
-        <v>45</v>
+      <c r="G35" s="96" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4260,42 +4370,42 @@
         <v>4</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F36" s="18">
         <v>1</v>
       </c>
-      <c r="G36" s="89"/>
+      <c r="G36" s="96"/>
     </row>
     <row r="37" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="F37" s="46">
+      <c r="A37" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="45">
         <v>2</v>
       </c>
-      <c r="G37" s="89"/>
+      <c r="G37" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -4322,130 +4432,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEB0282-3FC1-4781-9F0B-0FB6CE0BD470}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="81.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.19921875" customWidth="1"/>
+    <col min="3" max="3" width="81.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.95" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
       <c r="B5" s="29"/>
       <c r="C5" s="21"/>
     </row>
-    <row r="6" spans="1:3" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="27" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="38.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="36.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="B11" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="38.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>213</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4453,53 +4563,53 @@
         <v>9</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="29"/>
       <c r="C13" s="21"/>
     </row>
-    <row r="14" spans="1:3" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="98.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="99.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20"/>
       <c r="B16" s="29"/>
       <c r="C16" s="21"/>
     </row>
-    <row r="17" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="38.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4507,40 +4617,40 @@
         <v>4</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="86.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="104" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="104"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.95" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="105" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="91" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="91"/>
-    </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="92"/>
+      <c r="C21" s="105"/>
     </row>
     <row r="22" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>